<commit_message>
connected frontend with all restrictions
</commit_message>
<xml_diff>
--- a/pyver/data/placement.xlsx
+++ b/pyver/data/placement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\DATA_SETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eenad\Downloads\CIET-CB\pyver\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6435842E-76E9-40F6-B076-4B4D7AD5630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAD94DB-5178-45A4-B350-D9E0DAA16908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="192">
   <si>
     <t>Venkata Vikas Bathula</t>
   </si>
@@ -548,9 +548,6 @@
   </si>
   <si>
     <t>Muddana Pragathi</t>
-  </si>
-  <si>
-    <t>Learnflu</t>
   </si>
   <si>
     <t>Netlync Technologies</t>
@@ -762,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1072,34 +1069,34 @@
   <dimension ref="A1:E197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D197"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="92.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="92.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1111,9 +1108,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -1125,9 +1122,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>2</v>
@@ -1139,9 +1136,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -1153,9 +1150,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -1167,9 +1164,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
@@ -1181,9 +1178,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -1195,9 +1192,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
@@ -1209,9 +1206,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
@@ -1223,9 +1220,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>9</v>
@@ -1237,9 +1234,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>10</v>
@@ -1251,9 +1248,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -1265,9 +1262,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>12</v>
@@ -1279,9 +1276,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>13</v>
@@ -1293,9 +1290,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1307,9 +1304,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>15</v>
@@ -1321,9 +1318,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>16</v>
@@ -1335,9 +1332,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>17</v>
@@ -1349,9 +1346,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>18</v>
@@ -1363,9 +1360,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>19</v>
@@ -1377,9 +1374,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>20</v>
@@ -1391,9 +1388,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>21</v>
@@ -1405,9 +1402,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>22</v>
@@ -1419,9 +1416,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>23</v>
@@ -1433,9 +1430,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>24</v>
@@ -1447,9 +1444,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>25</v>
@@ -1461,9 +1458,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>26</v>
@@ -1475,9 +1472,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>27</v>
@@ -1489,9 +1486,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>28</v>
@@ -1503,9 +1500,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>29</v>
@@ -1517,9 +1514,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>30</v>
@@ -1531,9 +1528,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>31</v>
@@ -1545,9 +1542,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>32</v>
@@ -1559,9 +1556,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>33</v>
@@ -1573,9 +1570,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>34</v>
@@ -1587,9 +1584,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>35</v>
@@ -1601,9 +1598,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>169</v>
@@ -1615,9 +1612,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>36</v>
@@ -1629,9 +1626,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>37</v>
@@ -1643,9 +1640,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>38</v>
@@ -1657,9 +1654,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>39</v>
@@ -1671,9 +1668,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>40</v>
@@ -1685,9 +1682,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>41</v>
@@ -1699,9 +1696,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>42</v>
@@ -1713,9 +1710,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>43</v>
@@ -1727,9 +1724,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>44</v>
@@ -1741,9 +1738,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>45</v>
@@ -1755,9 +1752,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>8</v>
@@ -1769,9 +1766,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>46</v>
@@ -1783,9 +1780,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>47</v>
@@ -1797,9 +1794,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>48</v>
@@ -1811,9 +1808,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>49</v>
@@ -1825,9 +1822,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>50</v>
@@ -1839,9 +1836,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>51</v>
@@ -1853,9 +1850,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>52</v>
@@ -1867,9 +1864,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>53</v>
@@ -1881,9 +1878,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>54</v>
@@ -1895,9 +1892,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>55</v>
@@ -1909,9 +1906,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>56</v>
@@ -1923,9 +1920,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>54</v>
@@ -1937,9 +1934,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>57</v>
@@ -1951,9 +1948,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>58</v>
@@ -1965,9 +1962,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>59</v>
@@ -1979,9 +1976,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>60</v>
@@ -1993,9 +1990,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>61</v>
@@ -2007,9 +2004,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>62</v>
@@ -2021,9 +2018,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>63</v>
@@ -2035,9 +2032,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>64</v>
@@ -2049,9 +2046,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>65</v>
@@ -2063,9 +2060,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>66</v>
@@ -2077,9 +2074,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>67</v>
@@ -2091,9 +2088,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>68</v>
@@ -2105,9 +2102,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>69</v>
@@ -2119,9 +2116,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>170</v>
@@ -2133,9 +2130,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>70</v>
@@ -2147,9 +2144,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>71</v>
@@ -2161,9 +2158,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>72</v>
@@ -2175,9 +2172,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>73</v>
@@ -2189,9 +2186,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>46</v>
@@ -2203,9 +2200,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>74</v>
@@ -2217,9 +2214,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>75</v>
@@ -2231,9 +2228,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>76</v>
@@ -2245,9 +2242,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>77</v>
@@ -2259,9 +2256,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>78</v>
@@ -2273,9 +2270,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>79</v>
@@ -2287,9 +2284,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>80</v>
@@ -2301,9 +2298,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>81</v>
@@ -2315,9 +2312,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>82</v>
@@ -2329,9 +2326,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>83</v>
@@ -2343,9 +2340,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>84</v>
@@ -2357,9 +2354,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>85</v>
@@ -2371,9 +2368,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>86</v>
@@ -2385,9 +2382,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>87</v>
@@ -2399,9 +2396,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>88</v>
@@ -2413,9 +2410,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>89</v>
@@ -2427,9 +2424,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>90</v>
@@ -2441,9 +2438,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>91</v>
@@ -2455,9 +2452,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>92</v>
@@ -2469,9 +2466,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>93</v>
@@ -2483,9 +2480,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>8</v>
@@ -2497,9 +2494,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>94</v>
@@ -2511,9 +2508,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>95</v>
@@ -2525,9 +2522,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>6</v>
@@ -2539,9 +2536,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>96</v>
@@ -2553,9 +2550,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>97</v>
@@ -2567,9 +2564,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>98</v>
@@ -2581,9 +2578,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>99</v>
@@ -2595,9 +2592,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>100</v>
@@ -2609,9 +2606,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>101</v>
@@ -2623,12 +2620,12 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>159</v>
@@ -2637,52 +2634,52 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="3" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" s="3" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>171</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="D112" s="4">
         <v>2025</v>
       </c>
       <c r="E112" s="2"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D113" s="4">
         <v>2025</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D114" s="4">
         <v>2025</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>102</v>
@@ -2694,9 +2691,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>103</v>
@@ -2708,9 +2705,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>5</v>
@@ -2722,9 +2719,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>104</v>
@@ -2736,9 +2733,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>105</v>
@@ -2750,9 +2747,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>106</v>
@@ -2764,9 +2761,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>107</v>
@@ -2778,9 +2775,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>108</v>
@@ -2792,9 +2789,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>109</v>
@@ -2806,9 +2803,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>110</v>
@@ -2820,9 +2817,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>1</v>
@@ -2834,9 +2831,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>111</v>
@@ -2848,9 +2845,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>56</v>
@@ -2862,9 +2859,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>112</v>
@@ -2876,9 +2873,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>113</v>
@@ -2890,9 +2887,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>114</v>
@@ -2904,9 +2901,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>104</v>
@@ -2918,9 +2915,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>115</v>
@@ -2932,9 +2929,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>116</v>
@@ -2946,9 +2943,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>117</v>
@@ -2960,9 +2957,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>5</v>
@@ -2974,9 +2971,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>118</v>
@@ -2988,9 +2985,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>96</v>
@@ -3002,9 +2999,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>119</v>
@@ -3016,37 +3013,37 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>120</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D139" s="4">
         <v>2025</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D140" s="4">
         <v>2025</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>121</v>
@@ -3058,9 +3055,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>122</v>
@@ -3072,9 +3069,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>123</v>
@@ -3086,9 +3083,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>124</v>
@@ -3100,9 +3097,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>88</v>
@@ -3114,9 +3111,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>125</v>
@@ -3128,9 +3125,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>126</v>
@@ -3142,9 +3139,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>96</v>
@@ -3156,9 +3153,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>56</v>
@@ -3170,9 +3167,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>54</v>
@@ -3184,9 +3181,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>103</v>
@@ -3198,9 +3195,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>124</v>
@@ -3212,9 +3209,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B153" s="5" t="s">
         <v>4</v>
@@ -3226,9 +3223,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>127</v>
@@ -3240,9 +3237,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>5</v>
@@ -3254,9 +3251,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>128</v>
@@ -3268,9 +3265,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>129</v>
@@ -3282,9 +3279,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>130</v>
@@ -3296,9 +3293,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>131</v>
@@ -3310,9 +3307,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>132</v>
@@ -3324,9 +3321,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>65</v>
@@ -3338,9 +3335,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>133</v>
@@ -3352,9 +3349,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>71</v>
@@ -3366,9 +3363,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>134</v>
@@ -3380,9 +3377,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>98</v>
@@ -3394,9 +3391,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>135</v>
@@ -3408,9 +3405,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>136</v>
@@ -3422,9 +3419,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>54</v>
@@ -3436,9 +3433,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>47</v>
@@ -3450,9 +3447,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>104</v>
@@ -3464,9 +3461,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>137</v>
@@ -3478,9 +3475,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>138</v>
@@ -3492,9 +3489,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>139</v>
@@ -3506,9 +3503,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>140</v>
@@ -3520,9 +3517,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>141</v>
@@ -3534,9 +3531,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>86</v>
@@ -3548,9 +3545,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B177" s="5" t="s">
         <v>142</v>
@@ -3562,9 +3559,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B178" s="5" t="s">
         <v>143</v>
@@ -3576,9 +3573,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B179" s="5" t="s">
         <v>144</v>
@@ -3590,9 +3587,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B180" s="5" t="s">
         <v>145</v>
@@ -3604,9 +3601,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>146</v>
@@ -3618,9 +3615,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B182" s="5" t="s">
         <v>147</v>
@@ -3632,9 +3629,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B183" s="5" t="s">
         <v>148</v>
@@ -3646,9 +3643,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B184" s="5" t="s">
         <v>67</v>
@@ -3660,37 +3657,37 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B185" s="5" t="s">
         <v>149</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D185" s="4">
         <v>2025</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D186" s="4">
         <v>2025</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B187" s="5" t="s">
         <v>1</v>
@@ -3702,9 +3699,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B188" s="5" t="s">
         <v>51</v>
@@ -3716,9 +3713,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>150</v>
@@ -3730,9 +3727,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B190" s="5" t="s">
         <v>151</v>
@@ -3744,9 +3741,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B191" s="5" t="s">
         <v>152</v>
@@ -3758,9 +3755,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>153</v>
@@ -3772,9 +3769,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B193" s="5" t="s">
         <v>100</v>
@@ -3786,9 +3783,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B194" s="5" t="s">
         <v>101</v>
@@ -3800,12 +3797,12 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>166</v>
@@ -3814,9 +3811,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B196" s="5" t="s">
         <v>131</v>
@@ -3828,9 +3825,9 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>134</v>

</xml_diff>